<commit_message>
mostly final product and instructions
</commit_message>
<xml_diff>
--- a/Information/mappingVolMonDB_AWQMS.xlsx
+++ b/Information/mappingVolMonDB_AWQMS.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="78">
   <si>
     <t>t_Activity</t>
   </si>
@@ -201,21 +201,6 @@
     <t>join to tlu_Stations</t>
   </si>
   <si>
-    <t>recode import config? Or join to tlu_TimeZones</t>
-  </si>
-  <si>
-    <t>recode import config? Or join to tlu_units</t>
-  </si>
-  <si>
-    <t>recode import config? Or join to tlu_Characteristic</t>
-  </si>
-  <si>
-    <t>recode import config? tlu_Method</t>
-  </si>
-  <si>
-    <t>recode import config? Or join to tlu_Type</t>
-  </si>
-  <si>
     <t>join to tlu_Organization</t>
   </si>
   <si>
@@ -243,22 +228,37 @@
     <t>PrecisionValue</t>
   </si>
   <si>
-    <t>StatisticalBasis</t>
-  </si>
-  <si>
     <t>RsltTimeBasis</t>
   </si>
   <si>
     <t>import config deals with this</t>
   </si>
   <si>
-    <t>DEQ_PREC</t>
-  </si>
-  <si>
     <t>SmplColEquipComment</t>
   </si>
   <si>
     <t>recoded import config</t>
+  </si>
+  <si>
+    <t>join to tlu_units</t>
+  </si>
+  <si>
+    <t>join to tlu_Method</t>
+  </si>
+  <si>
+    <t>Org_RsltComment</t>
+  </si>
+  <si>
+    <t>StatisticalBasisID</t>
+  </si>
+  <si>
+    <t>join to tlu_Characteristic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does this need a translation? </t>
+  </si>
+  <si>
+    <t>ORDEQ_DQL</t>
   </si>
 </sst>
 </file>
@@ -281,18 +281,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -309,8 +303,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -745,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,7 +772,7 @@
         <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -825,7 +819,7 @@
         <v>41</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -861,7 +855,7 @@
         <v>44</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -872,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -897,7 +891,7 @@
         <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -922,7 +916,7 @@
         <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -947,7 +941,7 @@
         <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -961,7 +955,7 @@
         <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -986,73 +980,79 @@
         <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
+      <c r="D20" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
-        <v>65</v>
+      <c r="B23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" t="s">
-        <v>66</v>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -1063,10 +1063,10 @@
         <v>49</v>
       </c>
       <c r="C26" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -1077,7 +1077,10 @@
         <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>68</v>
+        <v>63</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -1087,8 +1090,8 @@
       <c r="B28" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>69</v>
+      <c r="C28" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1099,7 +1102,7 @@
         <v>49</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1109,8 +1112,8 @@
       <c r="B30" t="s">
         <v>49</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>70</v>
+      <c r="C30" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1120,8 +1123,8 @@
       <c r="B31" t="s">
         <v>49</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>71</v>
+      <c r="C31" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -1131,38 +1134,47 @@
       <c r="B32" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>